<commit_message>
Criamos no DFD o processo "Realizar entrega" derivado do "Realizar pedido". Revisado itens que não estavam mais nos DFD mas ainda constavam no arquivo. Atualização do eventos devido a alteração no EA.
</commit_message>
<xml_diff>
--- a/ModelagemProcessosNegocio/Impacta-es13-mpn-AnaliseEventosCenario.xlsx
+++ b/ModelagemProcessosNegocio/Impacta-es13-mpn-AnaliseEventosCenario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\Impacta\Repositórios\Impacta-es13-tcc-grupo01.github.io\ModelagemProcessosNegocio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\Impacta\Repositórios\Impacta-es13-tcc-grupo01.github.io.git\ModelagemProcessosNegocio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="32">
   <si>
     <t>Externo</t>
   </si>
@@ -104,12 +104,6 @@
     <t>FA</t>
   </si>
   <si>
-    <t>X(3)</t>
-  </si>
-  <si>
-    <t>Vendas</t>
-  </si>
-  <si>
     <t>Atendente envia catálogos</t>
   </si>
   <si>
@@ -128,15 +122,9 @@
     <t>Atendente confere pedido</t>
   </si>
   <si>
-    <t>X(4)</t>
-  </si>
-  <si>
     <t>Entregador entrega o pedido</t>
   </si>
   <si>
-    <t>X(5)</t>
-  </si>
-  <si>
     <t>Cliente cancela pedido</t>
   </si>
   <si>
@@ -159,6 +147,12 @@
   </si>
   <si>
     <t>Fornecedor não entrega produtos</t>
+  </si>
+  <si>
+    <t>Realizar Vendas</t>
+  </si>
+  <si>
+    <t>Realizar Entregas</t>
   </si>
 </sst>
 </file>
@@ -216,7 +210,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,8 +247,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -421,15 +421,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -461,6 +504,37 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
@@ -470,70 +544,67 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -814,15 +885,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9" style="29"/>
+    <col min="3" max="3" width="9" style="15"/>
     <col min="4" max="4" width="46.25" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.25" customWidth="1"/>
@@ -830,344 +901,364 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="17"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="20" t="s">
+      <c r="A1" s="2"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="20" t="s">
+      <c r="F1" s="30"/>
+      <c r="G1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="22"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="4"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="23" t="s">
+      <c r="A2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="5" t="s">
+      <c r="B2" s="33"/>
+      <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="J2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6">
+        <v>1</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="9"/>
+    </row>
+    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="23"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="6">
+        <v>2</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="9"/>
+    </row>
+    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="6">
+        <v>3</v>
+      </c>
+      <c r="D5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="9"/>
+    </row>
+    <row r="6" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="23"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="6">
+        <v>4</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="9"/>
+    </row>
+    <row r="7" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="23"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="6">
+        <v>5</v>
+      </c>
+      <c r="D7" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="23"/>
+      <c r="B8" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="41"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="7"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="9"/>
+    </row>
+    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="23"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="9"/>
+    </row>
+    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="23"/>
+      <c r="B10" s="25"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="13"/>
+      <c r="I10" s="13"/>
+      <c r="J10" s="14"/>
+    </row>
+    <row r="11" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C11" s="40">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="D11" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" s="35"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9"/>
-      <c r="I3" s="9"/>
-      <c r="J3" s="10"/>
-    </row>
-    <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="15"/>
-      <c r="C4" s="7">
+      <c r="I11" s="13"/>
+      <c r="J11" s="14"/>
+    </row>
+    <row r="12" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="39"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="40">
         <v>2</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="H4" s="9"/>
-      <c r="I4" s="9"/>
-      <c r="J4" s="10"/>
-    </row>
-    <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="7">
+      <c r="I12" s="13"/>
+      <c r="J12" s="14"/>
+    </row>
+    <row r="13" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="40">
         <v>3</v>
       </c>
-      <c r="D5" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="D13" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="35"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="I13" s="13"/>
+      <c r="J13" s="14"/>
+    </row>
+    <row r="14" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="39"/>
+      <c r="B14" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40"/>
+      <c r="E14" s="35"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="13"/>
+      <c r="H14" s="13"/>
+      <c r="I14" s="13"/>
+      <c r="J14" s="14"/>
+    </row>
+    <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="38">
+        <v>1</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="7"/>
+      <c r="F15" s="7"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="9"/>
-      <c r="I5" s="9"/>
-      <c r="J5" s="10"/>
-    </row>
-    <row r="6" spans="1:10" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="7">
+      <c r="I15" s="8"/>
+      <c r="J15" s="9"/>
+    </row>
+    <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="21"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="18">
+        <v>2</v>
+      </c>
+      <c r="D16" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="8"/>
+      <c r="J16" s="9"/>
+    </row>
+    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="18">
+        <v>3</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="I17" s="8"/>
+      <c r="J17" s="9"/>
+    </row>
+    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21"/>
+      <c r="B18" s="20"/>
+      <c r="C18" s="18">
         <v>4</v>
       </c>
-      <c r="D6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="I6" s="9"/>
-      <c r="J6" s="10"/>
-    </row>
-    <row r="7" spans="1:10" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="7">
+      <c r="D18" s="16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21"/>
+      <c r="B19" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="19">
         <v>5</v>
       </c>
-      <c r="D7" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="9"/>
-      <c r="J7" s="10"/>
-    </row>
-    <row r="8" spans="1:10" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="7">
-        <v>6</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="9"/>
-      <c r="H8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="I8" s="9"/>
-      <c r="J8" s="10"/>
-    </row>
-    <row r="9" spans="1:10" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="7">
-        <v>7</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="D19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="10"/>
-    </row>
-    <row r="10" spans="1:10" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="16"/>
-      <c r="C10" s="7">
-        <v>8</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="10"/>
-    </row>
-    <row r="11" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
-      <c r="B11" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="7"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="9"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="10"/>
-    </row>
-    <row r="12" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="9"/>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="10"/>
-    </row>
-    <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
-      <c r="B13" s="15"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="26"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
-      <c r="J13" s="28"/>
-    </row>
-    <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="32" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" s="33" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14" s="35">
-        <v>1</v>
-      </c>
-      <c r="D14" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="9"/>
-      <c r="H14" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="I14" s="9"/>
-      <c r="J14" s="10"/>
-    </row>
-    <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
-      <c r="C15" s="36">
-        <v>2</v>
-      </c>
-      <c r="D15" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="10"/>
-    </row>
-    <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
-      <c r="C16" s="36">
-        <v>3</v>
-      </c>
-      <c r="D16" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="10"/>
-    </row>
-    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
-      <c r="C17" s="36">
-        <v>4</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="37">
-        <v>5</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="9"/>
-      <c r="I18" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="10"/>
+      <c r="J19" s="9"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="A3:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B1:D1"/>
+  <mergeCells count="11">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="B3:B10"/>
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Correção ortográfica RN-12 Correção evento n°5 Realizar compras
</commit_message>
<xml_diff>
--- a/ModelagemProcessosNegocio/Impacta-es13-mpn-AnaliseEventosCenario.xlsx
+++ b/ModelagemProcessosNegocio/Impacta-es13-mpn-AnaliseEventosCenario.xlsx
@@ -143,9 +143,6 @@
     <t>Diretor calcula média de vendas</t>
   </si>
   <si>
-    <t>Fornecedor não entrega produtos</t>
-  </si>
-  <si>
     <t>Realizar Entregas</t>
   </si>
   <si>
@@ -153,6 +150,9 @@
   </si>
   <si>
     <t>Realizar Compras</t>
+  </si>
+  <si>
+    <t>Atendente cobra fornecedor</t>
   </si>
 </sst>
 </file>
@@ -551,6 +551,39 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -566,44 +599,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -891,7 +891,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B1" sqref="B1:D1"/>
+      <selection pane="bottomRight" activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -905,25 +905,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="40" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="41"/>
+      <c r="G1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="41"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="44"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -950,10 +950,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="33" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="35" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6">
@@ -972,8 +972,8 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="36"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -990,8 +990,8 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="36"/>
       <c r="C5" s="6">
         <v>3</v>
       </c>
@@ -1008,8 +1008,8 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="36"/>
       <c r="C6" s="6">
         <v>4</v>
       </c>
@@ -1026,8 +1026,8 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="34"/>
+      <c r="B7" s="45"/>
       <c r="C7" s="6">
         <v>5</v>
       </c>
@@ -1044,8 +1044,8 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="34"/>
+      <c r="B8" s="35" t="s">
         <v>14</v>
       </c>
       <c r="C8" s="23"/>
@@ -1058,8 +1058,8 @@
       <c r="J8" s="9"/>
     </row>
     <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="36"/>
       <c r="C9" s="23"/>
       <c r="D9" s="28"/>
       <c r="E9" s="25"/>
@@ -1070,8 +1070,8 @@
       <c r="J9" s="9"/>
     </row>
     <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="35"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="24"/>
       <c r="D10" s="28"/>
       <c r="E10" s="20"/>
@@ -1082,10 +1082,10 @@
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="B11" s="37" t="s">
+      <c r="A11" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="30" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="22">
@@ -1104,8 +1104,8 @@
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="46"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="22">
         <v>2</v>
       </c>
@@ -1122,8 +1122,8 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="37"/>
+      <c r="A13" s="46"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="22">
         <v>3</v>
       </c>
@@ -1140,7 +1140,7 @@
       <c r="J13" s="14"/>
     </row>
     <row r="14" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
+      <c r="A14" s="46"/>
       <c r="B14" s="17" t="s">
         <v>14</v>
       </c>
@@ -1154,10 +1154,10 @@
       <c r="J14" s="14"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
-        <v>31</v>
-      </c>
-      <c r="B15" s="39" t="s">
+      <c r="A15" s="31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="29" t="s">
         <v>11</v>
       </c>
       <c r="C15" s="21">
@@ -1176,8 +1176,8 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="18">
         <v>2</v>
       </c>
@@ -1194,8 +1194,8 @@
       <c r="J16" s="9"/>
     </row>
     <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="30"/>
       <c r="C17" s="18">
         <v>3</v>
       </c>
@@ -1212,8 +1212,8 @@
       <c r="J17" s="9"/>
     </row>
     <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="37"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="30"/>
       <c r="C18" s="18">
         <v>4</v>
       </c>
@@ -1230,7 +1230,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
+      <c r="A19" s="32"/>
       <c r="B19" s="17" t="s">
         <v>14</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>5</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -1251,17 +1251,17 @@
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B1:D1"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B7"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A3:A10"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Definição do cenário de compras
</commit_message>
<xml_diff>
--- a/ModelagemProcessosNegocio/Impacta-es13-mpn-AnaliseEventosCenario.xlsx
+++ b/ModelagemProcessosNegocio/Impacta-es13-mpn-AnaliseEventosCenario.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1600342\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ricardo\Documents\Impacta\Repositórios\Impacta-es13-tcc-grupo01.github.io.git\ModelagemProcessosNegocio\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>Externo</t>
   </si>
@@ -134,28 +134,43 @@
     <t>Diretor faz lista de compras</t>
   </si>
   <si>
-    <t>Diretor faz pedido de produtos</t>
-  </si>
-  <si>
     <t>Atendente recebe os produtos</t>
   </si>
   <si>
-    <t>Diretor calcula média de vendas</t>
-  </si>
-  <si>
     <t>Realizar Entregas</t>
   </si>
   <si>
     <t>Realizar Pedidos</t>
   </si>
   <si>
-    <t>Realizar Compras</t>
-  </si>
-  <si>
-    <t>Atendente cobra fornecedor</t>
-  </si>
-  <si>
     <t>X(3)</t>
+  </si>
+  <si>
+    <t>Diretor envia solicitação de produtos</t>
+  </si>
+  <si>
+    <t>Diretor cadastra novo fornecedor</t>
+  </si>
+  <si>
+    <t>Atendente cadastra produto</t>
+  </si>
+  <si>
+    <t>Atualizar produtos</t>
+  </si>
+  <si>
+    <t>X(4)</t>
+  </si>
+  <si>
+    <t>FALHA</t>
+  </si>
+  <si>
+    <t>Atendente cobra catálogos fornecedor</t>
+  </si>
+  <si>
+    <t>Atendente cobra pedidos fornecedor</t>
+  </si>
+  <si>
+    <t>Realizar compras</t>
   </si>
 </sst>
 </file>
@@ -436,19 +451,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right style="thin">
         <color indexed="64"/>
@@ -461,12 +463,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FF000000"/>
+        <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -474,7 +489,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -523,16 +538,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -541,9 +550,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -554,6 +560,36 @@
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -569,44 +605,36 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" textRotation="90" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -888,45 +916,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="9" style="15"/>
+    <col min="3" max="3" width="5.140625" style="15" customWidth="1"/>
     <col min="4" max="4" width="46.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
     <col min="9" max="9" width="13.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="29" t="s">
+      <c r="B1" s="33"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="30"/>
-      <c r="G1" s="29" t="s">
+      <c r="F1" s="37"/>
+      <c r="G1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="37"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="33"/>
+      <c r="B2" s="40"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -953,10 +982,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" s="34" t="s">
+      <c r="A3" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="31" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6">
@@ -975,8 +1004,8 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="35"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="32"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -993,8 +1022,8 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="43"/>
-      <c r="B5" s="35"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="32"/>
       <c r="C5" s="6">
         <v>3</v>
       </c>
@@ -1011,8 +1040,8 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="43"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="32"/>
       <c r="C6" s="6">
         <v>4</v>
       </c>
@@ -1020,7 +1049,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F6" s="7"/>
       <c r="G6" s="8"/>
@@ -1029,16 +1058,16 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="43"/>
-      <c r="B7" s="36"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="41"/>
       <c r="C7" s="6">
         <v>5</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="23" t="s">
         <v>22</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="8"/>
@@ -1047,224 +1076,255 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="43"/>
-      <c r="B8" s="34" t="s">
+      <c r="A8" s="30"/>
+      <c r="B8" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="23"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="25"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="25"/>
+      <c r="E8" s="22"/>
       <c r="F8" s="7"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
     </row>
-    <row r="9" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="43"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8"/>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9"/>
-    </row>
-    <row r="10" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="43"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="20"/>
+    <row r="9" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="42" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="20">
+        <v>1</v>
+      </c>
+      <c r="D9" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="18"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+      <c r="H9" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="13"/>
+      <c r="J9" s="14"/>
+    </row>
+    <row r="10" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="42"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="20">
+        <v>2</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="18"/>
       <c r="F10" s="12"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="H10" s="13" t="s">
+        <v>17</v>
+      </c>
       <c r="I10" s="13"/>
       <c r="J10" s="14"/>
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="37" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="22">
-        <v>1</v>
-      </c>
-      <c r="D11" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E11" s="20"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="20">
+        <v>3</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="18"/>
       <c r="F11" s="12"/>
       <c r="G11" s="13"/>
       <c r="H11" s="13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" s="13"/>
       <c r="J11" s="14"/>
     </row>
     <row r="12" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="38"/>
-      <c r="B12" s="37"/>
-      <c r="C12" s="22">
-        <v>2</v>
-      </c>
-      <c r="D12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" s="20"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="18"/>
       <c r="F12" s="12"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="13" t="s">
-        <v>17</v>
-      </c>
+      <c r="H12" s="13"/>
       <c r="I12" s="13"/>
       <c r="J12" s="14"/>
     </row>
-    <row r="13" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="38"/>
-      <c r="B13" s="37"/>
-      <c r="C13" s="22">
+    <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="51" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="19">
+        <v>1</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="22"/>
+      <c r="F13" s="7"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="51"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="19">
+        <v>2</v>
+      </c>
+      <c r="D14" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="51"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="19">
         <v>3</v>
       </c>
-      <c r="D13" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="20"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="I13" s="13"/>
-      <c r="J13" s="14"/>
-    </row>
-    <row r="14" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="38"/>
-      <c r="B14" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="14"/>
-    </row>
-    <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="40" t="s">
-        <v>30</v>
-      </c>
-      <c r="B15" s="39" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="21">
-        <v>1</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="7"/>
+      <c r="D15" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>12</v>
+      </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
-      <c r="H15" s="8" t="s">
-        <v>12</v>
-      </c>
+      <c r="H15" s="8"/>
       <c r="I15" s="8"/>
       <c r="J15" s="9"/>
     </row>
-    <row r="16" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="41"/>
-      <c r="B16" s="37"/>
-      <c r="C16" s="18">
-        <v>2</v>
-      </c>
-      <c r="D16" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="8"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="41"/>
-      <c r="B17" s="37"/>
-      <c r="C17" s="18">
-        <v>3</v>
-      </c>
-      <c r="D17" s="16" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="7"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="37"/>
-      <c r="C18" s="18">
+    <row r="16" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="51"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="19">
         <v>4</v>
       </c>
-      <c r="D18" s="16" t="s">
-        <v>27</v>
-      </c>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="9" t="s">
+      <c r="D16" s="44" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="45"/>
+      <c r="F16" s="45"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="47" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="41"/>
-      <c r="B19" s="17" t="s">
+    <row r="17" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="51"/>
+      <c r="B17" s="49"/>
+      <c r="C17" s="19">
+        <v>5</v>
+      </c>
+      <c r="D17" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="45"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
+      <c r="J17" s="47"/>
+    </row>
+    <row r="18" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="51"/>
+      <c r="B18" s="49"/>
+      <c r="C18" s="19">
+        <v>6</v>
+      </c>
+      <c r="D18" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="47"/>
+    </row>
+    <row r="19" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="51"/>
+      <c r="B19" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C19" s="19">
-        <v>5</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8" t="s">
+      <c r="C19" s="20">
+        <v>7</v>
+      </c>
+      <c r="D19" s="50" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="45"/>
+      <c r="F19" s="45"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="9"/>
+      <c r="J19" s="47"/>
+    </row>
+    <row r="20" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="51"/>
+      <c r="B20" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="43">
+        <v>8</v>
+      </c>
+      <c r="D20" s="50" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="45"/>
+      <c r="F20" s="45"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="J20" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="B15:B18"/>
-    <mergeCell ref="A15:A19"/>
-    <mergeCell ref="A3:A10"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B1:D1"/>
+  <mergeCells count="10">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="B3:B7"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="A11:A14"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A3:A8"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="B13:B18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Criado ciclo de vida da relação de de pedidos. Correção no item 3 do realizar compras
</commit_message>
<xml_diff>
--- a/ModelagemProcessosNegocio/Impacta-es13-mpn-AnaliseEventosCenario.xlsx
+++ b/ModelagemProcessosNegocio/Impacta-es13-mpn-AnaliseEventosCenario.xlsx
@@ -152,9 +152,6 @@
     <t>Diretor cadastra novo fornecedor</t>
   </si>
   <si>
-    <t>Atendente cadastra produto</t>
-  </si>
-  <si>
     <t>Atualizar produtos</t>
   </si>
   <si>
@@ -171,6 +168,9 @@
   </si>
   <si>
     <t>Realizar compras</t>
+  </si>
+  <si>
+    <t>Atendente cadastra produtos</t>
   </si>
 </sst>
 </file>
@@ -566,21 +566,55 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -590,39 +624,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
@@ -630,11 +633,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,10 +919,10 @@
   <dimension ref="A1:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="D14" sqref="D14"/>
+      <selection pane="bottomRight" activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -937,25 +937,25 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="36" t="s">
+      <c r="B1" s="45"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="33" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="37"/>
-      <c r="G1" s="36" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="37"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="34"/>
       <c r="J1" s="3"/>
     </row>
     <row r="2" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="40"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="4" t="s">
         <v>3</v>
       </c>
@@ -982,10 +982,10 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="38" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="6">
@@ -1004,8 +1004,8 @@
       <c r="J3" s="9"/>
     </row>
     <row r="4" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="32"/>
+      <c r="A4" s="44"/>
+      <c r="B4" s="39"/>
       <c r="C4" s="6">
         <v>2</v>
       </c>
@@ -1022,8 +1022,8 @@
       <c r="J4" s="9"/>
     </row>
     <row r="5" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30"/>
-      <c r="B5" s="32"/>
+      <c r="A5" s="44"/>
+      <c r="B5" s="39"/>
       <c r="C5" s="6">
         <v>3</v>
       </c>
@@ -1040,8 +1040,8 @@
       <c r="J5" s="9"/>
     </row>
     <row r="6" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30"/>
-      <c r="B6" s="32"/>
+      <c r="A6" s="44"/>
+      <c r="B6" s="39"/>
       <c r="C6" s="6">
         <v>4</v>
       </c>
@@ -1058,8 +1058,8 @@
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="30"/>
-      <c r="B7" s="41"/>
+      <c r="A7" s="44"/>
+      <c r="B7" s="40"/>
       <c r="C7" s="6">
         <v>5</v>
       </c>
@@ -1076,7 +1076,7 @@
       <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="30"/>
+      <c r="A8" s="44"/>
       <c r="B8" s="26" t="s">
         <v>14</v>
       </c>
@@ -1093,7 +1093,7 @@
       <c r="A9" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="28" t="s">
+      <c r="B9" s="41" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="20">
@@ -1113,7 +1113,7 @@
     </row>
     <row r="10" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="42"/>
-      <c r="B10" s="28"/>
+      <c r="B10" s="41"/>
       <c r="C10" s="20">
         <v>2</v>
       </c>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="11" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="42"/>
-      <c r="B11" s="28"/>
+      <c r="B11" s="41"/>
       <c r="C11" s="20">
         <v>3</v>
       </c>
@@ -1162,10 +1162,10 @@
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="51" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" s="48" t="s">
+      <c r="A13" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="49" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="19">
@@ -1184,8 +1184,8 @@
       <c r="J13" s="9"/>
     </row>
     <row r="14" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="51"/>
-      <c r="B14" s="49"/>
+      <c r="A14" s="48"/>
+      <c r="B14" s="50"/>
       <c r="C14" s="19">
         <v>2</v>
       </c>
@@ -1202,8 +1202,8 @@
       <c r="J14" s="9"/>
     </row>
     <row r="15" spans="1:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="51"/>
-      <c r="B15" s="49"/>
+      <c r="A15" s="48"/>
+      <c r="B15" s="50"/>
       <c r="C15" s="19">
         <v>3</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>25</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="F15" s="7"/>
       <c r="G15" s="8"/>
@@ -1220,101 +1220,103 @@
       <c r="J15" s="9"/>
     </row>
     <row r="16" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="51"/>
-      <c r="B16" s="49"/>
+      <c r="A16" s="48"/>
+      <c r="B16" s="50"/>
       <c r="C16" s="19">
         <v>4</v>
       </c>
-      <c r="D16" s="44" t="s">
+      <c r="D16" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="E16" s="45"/>
-      <c r="F16" s="45"/>
-      <c r="G16" s="46"/>
-      <c r="H16" s="46"/>
-      <c r="I16" s="46"/>
-      <c r="J16" s="47" t="s">
+      <c r="E16" s="29"/>
+      <c r="F16" s="29"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="51"/>
-      <c r="B17" s="49"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="50"/>
       <c r="C17" s="19">
         <v>5</v>
       </c>
-      <c r="D17" s="44" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46"/>
-      <c r="H17" s="46"/>
-      <c r="I17" s="46"/>
-      <c r="J17" s="47"/>
+      <c r="D17" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="29" t="s">
+        <v>32</v>
+      </c>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="31"/>
     </row>
     <row r="18" spans="1:10" s="1" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="51"/>
-      <c r="B18" s="49"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="50"/>
       <c r="C18" s="19">
         <v>6</v>
       </c>
-      <c r="D18" s="44" t="s">
-        <v>32</v>
-      </c>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45" t="s">
+      <c r="D18" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="29"/>
+      <c r="F18" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="G18" s="46"/>
-      <c r="H18" s="46"/>
-      <c r="I18" s="46"/>
-      <c r="J18" s="47"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
     </row>
     <row r="19" spans="1:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="51"/>
+      <c r="A19" s="48"/>
       <c r="B19" s="27" t="s">
         <v>14</v>
       </c>
       <c r="C19" s="20">
         <v>7</v>
       </c>
-      <c r="D19" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="45"/>
-      <c r="F19" s="45"/>
-      <c r="G19" s="46"/>
-      <c r="H19" s="46"/>
-      <c r="I19" s="46" t="s">
+      <c r="D19" s="32" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="29"/>
+      <c r="F19" s="29"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="J19" s="47"/>
+      <c r="J19" s="31"/>
     </row>
     <row r="20" spans="1:10" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="51"/>
+      <c r="A20" s="48"/>
       <c r="B20" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="51">
+        <v>8</v>
+      </c>
+      <c r="D20" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C20" s="43">
-        <v>8</v>
-      </c>
-      <c r="D20" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46" t="s">
+      <c r="E20" s="29"/>
+      <c r="F20" s="29"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="J20" s="47"/>
+      <c r="J20" s="31"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="B13:B18"/>
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="G1:I1"/>
     <mergeCell ref="A2:B2"/>
@@ -1323,8 +1325,6 @@
     <mergeCell ref="A9:A12"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="B1:D1"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="B13:B18"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>